<commit_message>
updated analysis to examine 10 crews, higher fid.
</commit_message>
<xml_diff>
--- a/Resilience Analysis/Acta/BPS/SparesDemand.xlsx
+++ b/Resilience Analysis/Acta/BPS/SparesDemand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16760" yWindow="0" windowWidth="16760" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33520" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="componentData.csv" sheetId="1" r:id="rId1"/>
@@ -900,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q94"/>
+  <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -911,7 +911,7 @@
     <col min="4" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -971,8 +971,23 @@
       <c r="L2">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="M2">
+        <v>52</v>
+      </c>
+      <c r="N2">
+        <v>60</v>
+      </c>
+      <c r="O2">
+        <v>69</v>
+      </c>
+      <c r="P2">
+        <v>78</v>
+      </c>
+      <c r="Q2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1003,8 +1018,23 @@
       <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1032,8 +1062,23 @@
       <c r="L4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -1064,8 +1109,23 @@
       <c r="L5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -1096,8 +1156,23 @@
       <c r="L6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -1128,8 +1203,23 @@
       <c r="L7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -1160,8 +1250,23 @@
       <c r="L8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="M8">
+        <v>13</v>
+      </c>
+      <c r="N8">
+        <v>15</v>
+      </c>
+      <c r="O8">
+        <v>17</v>
+      </c>
+      <c r="P8">
+        <v>19</v>
+      </c>
+      <c r="Q8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -1196,27 +1301,62 @@
         <v>2</v>
       </c>
       <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
         <f>H9+H18</f>
         <v>6</v>
       </c>
-      <c r="N9">
-        <f t="shared" ref="N9:Q9" si="0">I9+I18</f>
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="S9">
+        <f t="shared" ref="S9:AA17" si="0">I9+I18</f>
+        <v>4</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="C10" t="s">
         <v>18</v>
       </c>
@@ -1248,27 +1388,62 @@
         <v>2</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M17" si="1">H10+H19</f>
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ref="R10:R17" si="1">H10+H19</f>
         <v>8</v>
       </c>
-      <c r="N10">
-        <f t="shared" ref="N10:N17" si="2">I10+I19</f>
-        <v>2</v>
-      </c>
-      <c r="O10">
-        <f t="shared" ref="O10:O17" si="3">J10+J19</f>
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <f t="shared" ref="P10:Q17" si="4">K10+K19</f>
-        <v>4</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" ref="Q10:Q16" si="5">L10+L19</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="C11" t="s">
         <v>19</v>
       </c>
@@ -1297,27 +1472,62 @@
         <v>5</v>
       </c>
       <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N11">
-        <f t="shared" si="2"/>
+      <c r="S11">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O11">
-        <f t="shared" si="3"/>
+      <c r="T11">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="4"/>
+      <c r="U11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="Q11">
-        <f t="shared" si="5"/>
+      <c r="V11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="W11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
       <c r="C12" t="s">
         <v>20</v>
       </c>
@@ -1346,27 +1556,62 @@
         <v>5</v>
       </c>
       <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>6</v>
+      </c>
+      <c r="P12">
+        <v>7</v>
+      </c>
+      <c r="Q12">
+        <v>7</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="3"/>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="4"/>
+      <c r="U12">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="5"/>
+      <c r="V12">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="C13" t="s">
         <v>21</v>
       </c>
@@ -1395,27 +1640,62 @@
         <v>2</v>
       </c>
       <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="C14" t="s">
         <v>22</v>
       </c>
@@ -1447,27 +1727,62 @@
         <v>2</v>
       </c>
       <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="C15" t="s">
         <v>23</v>
       </c>
@@ -1496,27 +1811,62 @@
         <v>0</v>
       </c>
       <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="C16" t="s">
         <v>24</v>
       </c>
@@ -1548,27 +1898,62 @@
         <v>8</v>
       </c>
       <c r="M16">
+        <v>8</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <v>11</v>
+      </c>
+      <c r="P16">
+        <v>12</v>
+      </c>
+      <c r="Q16">
+        <v>12</v>
+      </c>
+      <c r="R16">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="2"/>
+      <c r="S16">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O16">
-        <f t="shared" si="3"/>
+      <c r="T16">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="4"/>
+      <c r="U16">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q16">
-        <f t="shared" si="5"/>
+      <c r="V16">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:17">
+      <c r="W16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27">
       <c r="C17" t="s">
         <v>25</v>
       </c>
@@ -1600,27 +1985,62 @@
         <v>5</v>
       </c>
       <c r="M17">
+        <v>8</v>
+      </c>
+      <c r="N17">
+        <v>12</v>
+      </c>
+      <c r="O17">
+        <v>14</v>
+      </c>
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <v>18</v>
+      </c>
+      <c r="R17">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="3"/>
+      <c r="S17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="4"/>
+      <c r="U17">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Q17">
-        <f t="shared" si="4"/>
+      <c r="V17">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:17">
+      <c r="W17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27">
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -1654,8 +2074,23 @@
       <c r="L18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:17">
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27">
       <c r="C19" t="s">
         <v>18</v>
       </c>
@@ -1686,8 +2121,23 @@
       <c r="L19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:17">
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27">
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -1715,8 +2165,23 @@
       <c r="L20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:17">
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>7</v>
+      </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27">
       <c r="C21" t="s">
         <v>20</v>
       </c>
@@ -1744,8 +2209,23 @@
       <c r="L21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:17">
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21">
+        <v>6</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+      <c r="Q21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27">
       <c r="C22" t="s">
         <v>21</v>
       </c>
@@ -1773,8 +2253,23 @@
       <c r="L22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:17">
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27">
       <c r="C23" t="s">
         <v>22</v>
       </c>
@@ -1805,8 +2300,23 @@
       <c r="L23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:17">
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27">
       <c r="C24" t="s">
         <v>23</v>
       </c>
@@ -1834,8 +2344,23 @@
       <c r="L24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:17">
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27">
       <c r="C25" t="s">
         <v>24</v>
       </c>
@@ -1866,8 +2391,23 @@
       <c r="L25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:17">
+      <c r="M25">
+        <v>8</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25">
+        <v>11</v>
+      </c>
+      <c r="P25">
+        <v>12</v>
+      </c>
+      <c r="Q25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27">
       <c r="C26" t="s">
         <v>25</v>
       </c>
@@ -1898,8 +2438,23 @@
       <c r="L26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="2:17">
+      <c r="M26">
+        <v>8</v>
+      </c>
+      <c r="N26">
+        <v>12</v>
+      </c>
+      <c r="O26">
+        <v>14</v>
+      </c>
+      <c r="P26">
+        <v>16</v>
+      </c>
+      <c r="Q26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -1930,8 +2485,23 @@
       <c r="L27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:17">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27">
       <c r="C28" t="s">
         <v>29</v>
       </c>
@@ -1959,8 +2529,23 @@
       <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:17">
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27">
       <c r="C29" t="s">
         <v>30</v>
       </c>
@@ -1988,8 +2573,23 @@
       <c r="L29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:17">
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27">
       <c r="C30" t="s">
         <v>31</v>
       </c>
@@ -2017,8 +2617,23 @@
       <c r="L30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:17">
+      <c r="M30">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27">
       <c r="C31" t="s">
         <v>32</v>
       </c>
@@ -2046,8 +2661,23 @@
       <c r="L31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="2:17">
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>3</v>
+      </c>
+      <c r="P31">
+        <v>4</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27">
       <c r="C32" t="s">
         <v>33</v>
       </c>
@@ -2078,8 +2708,23 @@
       <c r="L32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:12">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17">
       <c r="C33" t="s">
         <v>34</v>
       </c>
@@ -2107,8 +2752,23 @@
       <c r="L33">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="2:12">
+      <c r="M33">
+        <v>34</v>
+      </c>
+      <c r="N33">
+        <v>39</v>
+      </c>
+      <c r="O33">
+        <v>43</v>
+      </c>
+      <c r="P33">
+        <v>48</v>
+      </c>
+      <c r="Q33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17">
       <c r="C34" t="s">
         <v>35</v>
       </c>
@@ -2136,8 +2796,23 @@
       <c r="L34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:12">
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17">
       <c r="C35" t="s">
         <v>36</v>
       </c>
@@ -2168,8 +2843,23 @@
       <c r="L35">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="2:12">
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35">
+        <v>24</v>
+      </c>
+      <c r="O35">
+        <v>24</v>
+      </c>
+      <c r="P35">
+        <v>24</v>
+      </c>
+      <c r="Q35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17">
       <c r="C36" t="s">
         <v>37</v>
       </c>
@@ -2197,8 +2887,23 @@
       <c r="L36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="2:12">
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <v>2</v>
+      </c>
+      <c r="O36">
+        <v>3</v>
+      </c>
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17">
       <c r="B37" t="s">
         <v>38</v>
       </c>
@@ -2232,8 +2937,23 @@
       <c r="L37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="2:12">
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>7</v>
+      </c>
+      <c r="O37">
+        <v>8</v>
+      </c>
+      <c r="P37">
+        <v>9</v>
+      </c>
+      <c r="Q37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17">
       <c r="C38" t="s">
         <v>40</v>
       </c>
@@ -2264,8 +2984,23 @@
       <c r="L38">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="2:12">
+      <c r="M38">
+        <v>7</v>
+      </c>
+      <c r="N38">
+        <v>7</v>
+      </c>
+      <c r="O38">
+        <v>8</v>
+      </c>
+      <c r="P38">
+        <v>9</v>
+      </c>
+      <c r="Q38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17">
       <c r="C39" t="s">
         <v>41</v>
       </c>
@@ -2296,8 +3031,23 @@
       <c r="L39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="2:12">
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>3</v>
+      </c>
+      <c r="P39">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17">
       <c r="C40" t="s">
         <v>42</v>
       </c>
@@ -2328,8 +3078,23 @@
       <c r="L40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="2:12">
+      <c r="M40">
+        <v>6</v>
+      </c>
+      <c r="N40">
+        <v>7</v>
+      </c>
+      <c r="O40">
+        <v>8</v>
+      </c>
+      <c r="P40">
+        <v>9</v>
+      </c>
+      <c r="Q40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17">
       <c r="C41" t="s">
         <v>43</v>
       </c>
@@ -2360,8 +3125,23 @@
       <c r="L41">
         <v>135</v>
       </c>
-    </row>
-    <row r="42" spans="2:12">
+      <c r="M41">
+        <v>162</v>
+      </c>
+      <c r="N41">
+        <v>189</v>
+      </c>
+      <c r="O41">
+        <v>216</v>
+      </c>
+      <c r="P41">
+        <v>244</v>
+      </c>
+      <c r="Q41">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17">
       <c r="C42" t="s">
         <v>44</v>
       </c>
@@ -2392,8 +3172,23 @@
       <c r="L42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="2:12">
+      <c r="M42">
+        <v>13</v>
+      </c>
+      <c r="N42">
+        <v>15</v>
+      </c>
+      <c r="O42">
+        <v>17</v>
+      </c>
+      <c r="P42">
+        <v>19</v>
+      </c>
+      <c r="Q42">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17">
       <c r="B43" t="s">
         <v>45</v>
       </c>
@@ -2427,8 +3222,23 @@
       <c r="L43">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="2:12">
+      <c r="M43">
+        <v>7</v>
+      </c>
+      <c r="N43">
+        <v>8</v>
+      </c>
+      <c r="O43">
+        <v>8</v>
+      </c>
+      <c r="P43">
+        <v>10</v>
+      </c>
+      <c r="Q43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17">
       <c r="C44" t="s">
         <v>47</v>
       </c>
@@ -2459,8 +3269,23 @@
       <c r="L44">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="2:12">
+      <c r="M44">
+        <v>13</v>
+      </c>
+      <c r="N44">
+        <v>15</v>
+      </c>
+      <c r="O44">
+        <v>17</v>
+      </c>
+      <c r="P44">
+        <v>19</v>
+      </c>
+      <c r="Q44">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17">
       <c r="C45" t="s">
         <v>48</v>
       </c>
@@ -2491,8 +3316,23 @@
       <c r="L45">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="2:12">
+      <c r="M45">
+        <v>81</v>
+      </c>
+      <c r="N45">
+        <v>94</v>
+      </c>
+      <c r="O45">
+        <v>108</v>
+      </c>
+      <c r="P45">
+        <v>122</v>
+      </c>
+      <c r="Q45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17">
       <c r="C46" t="s">
         <v>49</v>
       </c>
@@ -2523,8 +3363,23 @@
       <c r="L46">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="2:12">
+      <c r="M46">
+        <v>13</v>
+      </c>
+      <c r="N46">
+        <v>15</v>
+      </c>
+      <c r="O46">
+        <v>17</v>
+      </c>
+      <c r="P46">
+        <v>19</v>
+      </c>
+      <c r="Q46">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17">
       <c r="C47" t="s">
         <v>50</v>
       </c>
@@ -2555,8 +3410,23 @@
       <c r="L47">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="2:12">
+      <c r="M47">
+        <v>36</v>
+      </c>
+      <c r="N47">
+        <v>42</v>
+      </c>
+      <c r="O47">
+        <v>48</v>
+      </c>
+      <c r="P47">
+        <v>54</v>
+      </c>
+      <c r="Q47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17">
       <c r="C48" t="s">
         <v>51</v>
       </c>
@@ -2587,8 +3457,23 @@
       <c r="L48">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="2:12">
+      <c r="M48">
+        <v>36</v>
+      </c>
+      <c r="N48">
+        <v>42</v>
+      </c>
+      <c r="O48">
+        <v>48</v>
+      </c>
+      <c r="P48">
+        <v>54</v>
+      </c>
+      <c r="Q48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17">
       <c r="C49" t="s">
         <v>52</v>
       </c>
@@ -2619,8 +3504,23 @@
       <c r="L49">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="2:12">
+      <c r="M49">
+        <v>59</v>
+      </c>
+      <c r="N49">
+        <v>69</v>
+      </c>
+      <c r="O49">
+        <v>78</v>
+      </c>
+      <c r="P49">
+        <v>88</v>
+      </c>
+      <c r="Q49">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17">
       <c r="C50" t="s">
         <v>53</v>
       </c>
@@ -2651,8 +3551,23 @@
       <c r="L50">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="2:12">
+      <c r="M50">
+        <v>13</v>
+      </c>
+      <c r="N50">
+        <v>15</v>
+      </c>
+      <c r="O50">
+        <v>17</v>
+      </c>
+      <c r="P50">
+        <v>19</v>
+      </c>
+      <c r="Q50">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17">
       <c r="C51" t="s">
         <v>14</v>
       </c>
@@ -2683,8 +3598,23 @@
       <c r="L51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="2:12">
+      <c r="M51">
+        <v>3</v>
+      </c>
+      <c r="N51">
+        <v>3</v>
+      </c>
+      <c r="O51">
+        <v>3</v>
+      </c>
+      <c r="P51">
+        <v>4</v>
+      </c>
+      <c r="Q51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17">
       <c r="C52" t="s">
         <v>54</v>
       </c>
@@ -2715,8 +3645,23 @@
       <c r="L52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="2:12">
+      <c r="M52">
+        <v>5</v>
+      </c>
+      <c r="N52">
+        <v>5</v>
+      </c>
+      <c r="O52">
+        <v>6</v>
+      </c>
+      <c r="P52">
+        <v>9</v>
+      </c>
+      <c r="Q52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17">
       <c r="C53" t="s">
         <v>55</v>
       </c>
@@ -2747,8 +3692,23 @@
       <c r="L53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="2:12">
+      <c r="M53">
+        <v>13</v>
+      </c>
+      <c r="N53">
+        <v>15</v>
+      </c>
+      <c r="O53">
+        <v>17</v>
+      </c>
+      <c r="P53">
+        <v>19</v>
+      </c>
+      <c r="Q53">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17">
       <c r="C54" t="s">
         <v>56</v>
       </c>
@@ -2779,8 +3739,23 @@
       <c r="L54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="2:12">
+      <c r="M54">
+        <v>2</v>
+      </c>
+      <c r="N54">
+        <v>2</v>
+      </c>
+      <c r="O54">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>2</v>
+      </c>
+      <c r="Q54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17">
       <c r="C55" t="s">
         <v>57</v>
       </c>
@@ -2811,8 +3786,23 @@
       <c r="L55">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="2:12">
+      <c r="M55">
+        <v>15</v>
+      </c>
+      <c r="N55">
+        <v>18</v>
+      </c>
+      <c r="O55">
+        <v>20</v>
+      </c>
+      <c r="P55">
+        <v>23</v>
+      </c>
+      <c r="Q55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17">
       <c r="C56" t="s">
         <v>58</v>
       </c>
@@ -2843,8 +3833,23 @@
       <c r="L56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="2:12">
+      <c r="M56">
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>2</v>
+      </c>
+      <c r="P56">
+        <v>2</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17">
       <c r="C57" t="s">
         <v>59</v>
       </c>
@@ -2875,8 +3880,23 @@
       <c r="L57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="2:12">
+      <c r="M57">
+        <v>3</v>
+      </c>
+      <c r="N57">
+        <v>4</v>
+      </c>
+      <c r="O57">
+        <v>4</v>
+      </c>
+      <c r="P57">
+        <v>4</v>
+      </c>
+      <c r="Q57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17">
       <c r="B58" t="s">
         <v>60</v>
       </c>
@@ -2907,8 +3927,23 @@
       <c r="L58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="2:12">
+      <c r="M58">
+        <v>5</v>
+      </c>
+      <c r="N58">
+        <v>4</v>
+      </c>
+      <c r="O58">
+        <v>5</v>
+      </c>
+      <c r="P58">
+        <v>5</v>
+      </c>
+      <c r="Q58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17">
       <c r="C59" t="s">
         <v>28</v>
       </c>
@@ -2936,8 +3971,23 @@
       <c r="L59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="2:12">
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17">
       <c r="C60" t="s">
         <v>62</v>
       </c>
@@ -2968,8 +4018,23 @@
       <c r="L60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="2:12">
+      <c r="M60">
+        <v>2</v>
+      </c>
+      <c r="N60">
+        <v>2</v>
+      </c>
+      <c r="O60">
+        <v>2</v>
+      </c>
+      <c r="P60">
+        <v>3</v>
+      </c>
+      <c r="Q60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17">
       <c r="C61" t="s">
         <v>63</v>
       </c>
@@ -3000,8 +4065,23 @@
       <c r="L61">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="2:12">
+      <c r="M61">
+        <v>10</v>
+      </c>
+      <c r="N61">
+        <v>12</v>
+      </c>
+      <c r="O61">
+        <v>12</v>
+      </c>
+      <c r="P61">
+        <v>13</v>
+      </c>
+      <c r="Q61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17">
       <c r="C62" t="s">
         <v>64</v>
       </c>
@@ -3032,8 +4112,23 @@
       <c r="L62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="2:12">
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
+      <c r="O62">
+        <v>3</v>
+      </c>
+      <c r="P62">
+        <v>2</v>
+      </c>
+      <c r="Q62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17">
       <c r="C63" t="s">
         <v>65</v>
       </c>
@@ -3064,8 +4159,23 @@
       <c r="L63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="2:12">
+      <c r="M63">
+        <v>3</v>
+      </c>
+      <c r="N63">
+        <v>2</v>
+      </c>
+      <c r="O63">
+        <v>3</v>
+      </c>
+      <c r="P63">
+        <v>3</v>
+      </c>
+      <c r="Q63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17">
       <c r="C64" t="s">
         <v>66</v>
       </c>
@@ -3093,8 +4203,23 @@
       <c r="L64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="M64">
+        <v>3</v>
+      </c>
+      <c r="N64">
+        <v>4</v>
+      </c>
+      <c r="O64">
+        <v>4</v>
+      </c>
+      <c r="P64">
+        <v>4</v>
+      </c>
+      <c r="Q64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
       <c r="B65" t="s">
         <v>67</v>
       </c>
@@ -3128,8 +4253,23 @@
       <c r="L65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="M65">
+        <v>2</v>
+      </c>
+      <c r="N65">
+        <v>2</v>
+      </c>
+      <c r="O65">
+        <v>2</v>
+      </c>
+      <c r="P65">
+        <v>2</v>
+      </c>
+      <c r="Q65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
       <c r="C66" t="s">
         <v>18</v>
       </c>
@@ -3160,8 +4300,23 @@
       <c r="L66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66">
+        <v>2</v>
+      </c>
+      <c r="N66">
+        <v>2</v>
+      </c>
+      <c r="O66">
+        <v>3</v>
+      </c>
+      <c r="P66">
+        <v>2</v>
+      </c>
+      <c r="Q66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
       <c r="C67" t="s">
         <v>19</v>
       </c>
@@ -3189,8 +4344,23 @@
       <c r="L67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="M67">
+        <v>6</v>
+      </c>
+      <c r="N67">
+        <v>6</v>
+      </c>
+      <c r="O67">
+        <v>7</v>
+      </c>
+      <c r="P67">
+        <v>7</v>
+      </c>
+      <c r="Q67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
       <c r="C68" t="s">
         <v>20</v>
       </c>
@@ -3218,8 +4388,23 @@
       <c r="L68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="M68">
+        <v>5</v>
+      </c>
+      <c r="N68">
+        <v>5</v>
+      </c>
+      <c r="O68">
+        <v>6</v>
+      </c>
+      <c r="P68">
+        <v>7</v>
+      </c>
+      <c r="Q68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
       <c r="C69" t="s">
         <v>21</v>
       </c>
@@ -3247,8 +4432,23 @@
       <c r="L69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69">
+        <v>2</v>
+      </c>
+      <c r="N69">
+        <v>3</v>
+      </c>
+      <c r="O69">
+        <v>2</v>
+      </c>
+      <c r="P69">
+        <v>3</v>
+      </c>
+      <c r="Q69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
       <c r="C70" t="s">
         <v>22</v>
       </c>
@@ -3279,8 +4479,23 @@
       <c r="L70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70">
+        <v>2</v>
+      </c>
+      <c r="N70">
+        <v>2</v>
+      </c>
+      <c r="O70">
+        <v>3</v>
+      </c>
+      <c r="P70">
+        <v>2</v>
+      </c>
+      <c r="Q70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
       <c r="C71" t="s">
         <v>23</v>
       </c>
@@ -3308,8 +4523,23 @@
       <c r="L71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="M71">
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <v>1</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
       <c r="C72" t="s">
         <v>24</v>
       </c>
@@ -3340,8 +4570,23 @@
       <c r="L72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="M72">
+        <v>8</v>
+      </c>
+      <c r="N72">
+        <v>10</v>
+      </c>
+      <c r="O72">
+        <v>11</v>
+      </c>
+      <c r="P72">
+        <v>12</v>
+      </c>
+      <c r="Q72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
       <c r="C73" t="s">
         <v>25</v>
       </c>
@@ -3372,8 +4617,23 @@
       <c r="L73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73">
+        <v>8</v>
+      </c>
+      <c r="N73">
+        <v>12</v>
+      </c>
+      <c r="O73">
+        <v>14</v>
+      </c>
+      <c r="P73">
+        <v>16</v>
+      </c>
+      <c r="Q73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
       <c r="C74" t="s">
         <v>68</v>
       </c>
@@ -3401,8 +4661,23 @@
       <c r="L74">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74">
+        <v>3</v>
+      </c>
+      <c r="N74">
+        <v>4</v>
+      </c>
+      <c r="O74">
+        <v>4</v>
+      </c>
+      <c r="P74">
+        <v>4</v>
+      </c>
+      <c r="Q74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
       <c r="B75" t="s">
         <v>69</v>
       </c>
@@ -3433,8 +4708,23 @@
       <c r="L75">
         <v>107</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="M75">
+        <v>125</v>
+      </c>
+      <c r="N75">
+        <v>145</v>
+      </c>
+      <c r="O75">
+        <v>163</v>
+      </c>
+      <c r="P75">
+        <v>182</v>
+      </c>
+      <c r="Q75">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>71</v>
       </c>
@@ -3468,8 +4758,23 @@
       <c r="L76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76">
+        <v>3</v>
+      </c>
+      <c r="N76">
+        <v>4</v>
+      </c>
+      <c r="O76">
+        <v>3</v>
+      </c>
+      <c r="P76">
+        <v>4</v>
+      </c>
+      <c r="Q76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
       <c r="C77" t="s">
         <v>66</v>
       </c>
@@ -3497,8 +4802,23 @@
       <c r="L77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="M77">
+        <v>5</v>
+      </c>
+      <c r="N77">
+        <v>7</v>
+      </c>
+      <c r="O77">
+        <v>7</v>
+      </c>
+      <c r="P77">
+        <v>7</v>
+      </c>
+      <c r="Q77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
       <c r="C78" t="s">
         <v>74</v>
       </c>
@@ -3526,8 +4846,23 @@
       <c r="L78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="M78">
+        <v>2</v>
+      </c>
+      <c r="N78">
+        <v>3</v>
+      </c>
+      <c r="O78">
+        <v>2</v>
+      </c>
+      <c r="P78">
+        <v>3</v>
+      </c>
+      <c r="Q78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17">
       <c r="B79" t="s">
         <v>75</v>
       </c>
@@ -3558,8 +4893,23 @@
       <c r="L79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>1</v>
+      </c>
+      <c r="O79">
+        <v>1</v>
+      </c>
+      <c r="P79">
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17">
       <c r="C80" t="s">
         <v>77</v>
       </c>
@@ -3587,8 +4937,23 @@
       <c r="L80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80">
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <v>1</v>
+      </c>
+      <c r="O80">
+        <v>1</v>
+      </c>
+      <c r="P80">
+        <v>1</v>
+      </c>
+      <c r="Q80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17">
       <c r="C81" t="s">
         <v>78</v>
       </c>
@@ -3616,8 +4981,23 @@
       <c r="L81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <v>1</v>
+      </c>
+      <c r="P81">
+        <v>1</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
       <c r="C82" t="s">
         <v>28</v>
       </c>
@@ -3645,8 +5025,23 @@
       <c r="L82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="M82">
+        <v>1</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>1</v>
+      </c>
+      <c r="P82">
+        <v>1</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
       <c r="C83" t="s">
         <v>79</v>
       </c>
@@ -3674,8 +5069,23 @@
       <c r="L83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="M83">
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <v>2</v>
+      </c>
+      <c r="O83">
+        <v>1</v>
+      </c>
+      <c r="P83">
+        <v>2</v>
+      </c>
+      <c r="Q83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -3709,8 +5119,23 @@
       <c r="L84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84">
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <v>1</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>1</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17">
       <c r="C85" t="s">
         <v>66</v>
       </c>
@@ -3738,8 +5163,23 @@
       <c r="L85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="M85">
+        <v>2</v>
+      </c>
+      <c r="N85">
+        <v>1</v>
+      </c>
+      <c r="O85">
+        <v>1</v>
+      </c>
+      <c r="P85">
+        <v>1</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17">
       <c r="C86" t="s">
         <v>74</v>
       </c>
@@ -3767,8 +5207,23 @@
       <c r="L86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="M86">
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+      <c r="P86">
+        <v>1</v>
+      </c>
+      <c r="Q86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
       <c r="B87" t="s">
         <v>75</v>
       </c>
@@ -3799,8 +5254,23 @@
       <c r="L87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>1</v>
+      </c>
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
       <c r="C88" t="s">
         <v>77</v>
       </c>
@@ -3828,8 +5298,23 @@
       <c r="L88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="N88">
+        <v>0</v>
+      </c>
+      <c r="O88">
+        <v>1</v>
+      </c>
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17">
       <c r="C89" t="s">
         <v>78</v>
       </c>
@@ -3857,8 +5342,23 @@
       <c r="L89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>1</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17">
       <c r="C90" t="s">
         <v>28</v>
       </c>
@@ -3886,8 +5386,23 @@
       <c r="L90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90">
+        <v>1</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
       <c r="C91" t="s">
         <v>79</v>
       </c>
@@ -3915,8 +5430,23 @@
       <c r="L91">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="M91">
+        <v>1</v>
+      </c>
+      <c r="N91">
+        <v>0</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -3937,6 +5467,21 @@
       </c>
       <c r="L94">
         <v>176</v>
+      </c>
+      <c r="M94">
+        <v>210</v>
+      </c>
+      <c r="N94">
+        <v>246</v>
+      </c>
+      <c r="O94">
+        <v>280</v>
+      </c>
+      <c r="P94">
+        <v>316</v>
+      </c>
+      <c r="Q94">
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>